<commit_message>
Fix Azure Calculator Source type
</commit_message>
<xml_diff>
--- a/Azure cost estimator.xlsx
+++ b/Azure cost estimator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgefree/Dropbox/opt/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFEA737-9B48-A046-A860-12D5C5422D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF270E6-8FA0-D04A-A118-4A0B31591319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Total annual cost</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/dynamodb/pricing/on-demand/</t>
-  </si>
-  <si>
     <t># sensors</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>Storage cost per GB (after 31 days)</t>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-us/pricing/details/cosmos-db/</t>
   </si>
 </sst>
 </file>
@@ -993,6 +993,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1003,8 +1005,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,8 +1417,8 @@
   </sheetPr>
   <dimension ref="B1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1440,7 +1440,7 @@
     <row r="4" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="4"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B8" s="88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="79"/>
       <c r="D8" s="80"/>
@@ -1465,18 +1465,18 @@
     <row r="9" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="83"/>
       <c r="C9" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="101"/>
+      <c r="C10" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="107"/>
-      <c r="C10" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="106">
+      <c r="D10" s="100">
         <v>0.12</v>
       </c>
     </row>
@@ -1485,13 +1485,13 @@
       <c r="C11" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="106">
+      <c r="D11" s="100">
         <v>2.76E-2</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B12" s="78" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="80"/>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="17" spans="2:30" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="51"/>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="21" spans="2:30" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B21" s="94" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="95"/>
       <c r="D21" s="96"/>
@@ -1705,38 +1705,35 @@
     </row>
     <row r="31" spans="2:30" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="62"/>
       <c r="D31" s="63"/>
     </row>
     <row r="32" spans="2:30" s="64" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="66"/>
       <c r="D32" s="67" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="64" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B33" s="68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="69"/>
       <c r="D33" s="70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D32" r:id="rId1" xr:uid="{4BD2BFD8-7227-B94E-932C-273D07D5DB4A}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1767,7 +1764,7 @@
     <row r="1" spans="2:33" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B2" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="21">
         <v>1000</v>
@@ -1811,21 +1808,21 @@
       <c r="AG2" s="2"/>
     </row>
     <row r="3" spans="2:33" ht="14" x14ac:dyDescent="0.15">
-      <c r="B3" s="100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="102"/>
+      <c r="B3" s="102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B4" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="25">
         <f>C2*(24*60/C47)*C44 / 1024 / 1024</f>
@@ -1853,7 +1850,7 @@
     </row>
     <row r="5" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B5" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="25">
         <f t="shared" ref="C5:G5" si="0">C4*7</f>
@@ -1881,7 +1878,7 @@
     </row>
     <row r="6" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B6" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="25">
         <f t="shared" ref="C6:G6" si="1">C5*7</f>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="7" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B7" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="25">
         <f t="shared" ref="C7:G7" si="2">C6*7</f>
@@ -1936,21 +1933,21 @@
       <c r="J7" s="23"/>
     </row>
     <row r="8" spans="2:33" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="100" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="102"/>
+      <c r="B8" s="102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="104"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B9" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="26">
         <f>C2*(24*60/C47)*C45</f>
@@ -1978,7 +1975,7 @@
     </row>
     <row r="10" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B10" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="26">
         <f t="shared" ref="C10:G10" si="3">C9*7</f>
@@ -2006,7 +2003,7 @@
     </row>
     <row r="11" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B11" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="26">
         <f t="shared" ref="C11:G11" si="4">C9*30</f>
@@ -2034,7 +2031,7 @@
     </row>
     <row r="12" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B12" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="26">
         <f t="shared" ref="C12:G12" si="5">C9*90</f>
@@ -2061,21 +2058,21 @@
       <c r="J12" s="23"/>
     </row>
     <row r="13" spans="2:33" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
+      <c r="B13" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="104"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
     </row>
     <row r="14" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="27">
         <f>(24*60/C47)*C2*C46</f>
@@ -2103,7 +2100,7 @@
     </row>
     <row r="15" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="28">
         <f t="shared" ref="C15:G15" si="6">C14*7</f>
@@ -2131,7 +2128,7 @@
     </row>
     <row r="16" spans="2:33" ht="15" x14ac:dyDescent="0.15">
       <c r="B16" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="28">
         <f t="shared" ref="C16:G16" si="7">C14*30</f>
@@ -2159,7 +2156,7 @@
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="29">
         <f t="shared" ref="C17:G17" si="8">C14*90</f>
@@ -2186,21 +2183,21 @@
       <c r="J17" s="23"/>
     </row>
     <row r="18" spans="2:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="100" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="102"/>
+      <c r="B18" s="102" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="104"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
     </row>
     <row r="19" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="32">
         <v>1.25</v>
@@ -2299,17 +2296,17 @@
       <c r="J26" s="23"/>
     </row>
     <row r="27" spans="2:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B27" s="104" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="105"/>
+      <c r="B27" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="107"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="23"/>
@@ -2335,7 +2332,7 @@
     </row>
     <row r="30" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B30" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
@@ -2447,7 +2444,7 @@
     </row>
     <row r="40" spans="2:10" ht="15" x14ac:dyDescent="0.15">
       <c r="B40" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="35">
         <v>0.15</v>
@@ -2462,7 +2459,7 @@
     </row>
     <row r="41" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B41" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="36">
         <v>0.03</v>
@@ -2477,7 +2474,7 @@
     </row>
     <row r="42" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B42" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="36">
         <v>0.5</v>
@@ -2492,7 +2489,7 @@
     </row>
     <row r="43" spans="2:10" ht="15" x14ac:dyDescent="0.15">
       <c r="B43" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="37">
         <v>5.0000000000000001E-3</v>
@@ -2507,7 +2504,7 @@
     </row>
     <row r="44" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B44" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" s="33">
         <v>150</v>
@@ -2522,7 +2519,7 @@
     </row>
     <row r="45" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B45" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="38">
         <f>C42/1024/1024/1024*C44</f>
@@ -2538,7 +2535,7 @@
     </row>
     <row r="46" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B46" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="39">
         <f>C41/1024/1024/1024*C44</f>
@@ -2554,7 +2551,7 @@
     </row>
     <row r="47" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B47" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="33">
         <v>5</v>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.15">
       <c r="B48" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" s="33">
         <v>7</v>
@@ -2626,7 +2623,7 @@
     <row r="4" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="2:29" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>